<commit_message>
adde ReadingExcel using method and try catch
</commit_message>
<xml_diff>
--- a/src/test/resources/CardDetails.xlsx
+++ b/src/test/resources/CardDetails.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>CardNumber</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Kuala Lumpur</t>
+  </si>
+  <si>
+    <t>V</t>
   </si>
 </sst>
 </file>
@@ -423,7 +426,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -467,6 +470,9 @@
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E2" s="1" t="s">
         <v>10</v>
       </c>

</xml_diff>